<commit_message>
Ajout de eventCode 9e8515c43121366088871f1d103d2d969e696dcc
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-Author.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-Author.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-30T07:06:28+00:00</t>
+    <t>2025-04-30T13:43:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,9 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>This Logical Mode describes the relevant attributes on the **Author** class within IHE ITI XDS.
-More details are to be retrieved from IHE ITI on www.ihe.net.
-(Focus for this LM is on the coded attributes.)</t>
+    <t>Model logique d'un auteur</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -1177,7 +1175,7 @@
         <v>73</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s" s="2">
         <v>72</v>
@@ -1250,7 +1248,7 @@
         <v>73</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AI6" t="s" s="2">
         <v>72</v>

</xml_diff>

<commit_message>
Ajout de l'authorPerson b45db128d703e5bc5c67fff9a7f91e49cc412255
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-Author.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-Author.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-02T14:15:44+00:00</t>
+    <t>2025-05-02T17:24:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -87,7 +87,8 @@
 - Un professionnel (personne physique) via son logiciel de professionnel, 
 - Le patient/usager (personne physique) via Mon espace Santé, 
 - Un système de structure (dispositif, automate, appareil connecté…), 
-- Un SNR (Service Numérique Référencé), </t>
+- Un SNR (Service Numérique Référencé), 
+author est un ensemble constitué des sous-attributs authorInstitution, authorPerson, authorRole et authorSpecialty et ne porte pas de valeur par lui-même. </t>
   </si>
   <si>
     <t>Purpose</t>
@@ -269,7 +270,7 @@
     <t>Author.person</t>
   </si>
   <si>
-    <t xml:space="preserve">https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/AuthorPerson
+    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/AuthorPersonPS|https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/AuthorPersonPatient|https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/AuthorPersonSNR|https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/AuthorPersonSystem)
 </t>
   </si>
   <si>
@@ -628,7 +629,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="67.8515625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Ajout du mapping 5b9ef178b55ff22959620fdaa372ac3e83db7c97
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-Author.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-Author.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="99">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-02T17:24:18+00:00</t>
+    <t>2025-05-03T11:17:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -238,6 +238,9 @@
     <t>Constraint(s)</t>
   </si>
   <si>
+    <t>Mapping: null</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -296,6 +299,12 @@
     <t>https://mos.esante.gouv.fr/NOS/JDV_J47-FunctionCode-CISIS/FHIR/JDV-J47-FunctionCode-CISIS</t>
   </si>
   <si>
+    <t>author/functionCode@displayName</t>
+  </si>
+  <si>
+    <t>Cet attribut n'a pas besoin d’être alimenté par un élément du DICOM KOS</t>
+  </si>
+  <si>
     <t>Author.specialty</t>
   </si>
   <si>
@@ -306,6 +315,12 @@
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J56-AuthorSpecialty-DMP/FHIR/JDV-J56-AuthorSpecialty-DMP</t>
+  </si>
+  <si>
+    <t>author/assignedAuthor/code@code</t>
+  </si>
+  <si>
+    <t>Cette métadonnée peut ne pas être renseignée dans le cas d’un DICOM KOS.   Si elle contient une valeur, elle devra contenir le code : 'DISPOSITIF' du JDV_J01_XdsAuthorSpecialty_CISIS</t>
   </si>
 </sst>
 </file>
@@ -610,7 +625,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -654,6 +669,8 @@
     <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
+    <col min="37" max="37" width="28.83984375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="146.93359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -765,6 +782,12 @@
       <c r="AJ1" t="s" s="1">
         <v>71</v>
       </c>
+      <c r="AK1" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="AL1" t="s" s="1">
+        <v>72</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
@@ -775,26 +798,26 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L2" t="s" s="2">
         <v>9</v>
@@ -805,461 +828,491 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AG2" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK2" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="AL2" t="s" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AL3" t="s" s="2">
+        <v>73</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AL4" t="s" s="2">
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Y5" s="2"/>
       <c r="Z5" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK5" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AL5" t="s" s="2">
+        <v>92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Y6" s="2"/>
       <c r="Z6" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AA6" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AB6" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AC6" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD6" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AE6" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AF6" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="AA6" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AB6" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AC6" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AD6" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AF6" t="s" s="2">
-        <v>90</v>
-      </c>
       <c r="AG6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK6" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="AL6" t="s" s="2">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout d'author dans le modele logique 6f6477248a1102d00e17cdcf4cd1d637abf50766
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-Author.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-Author.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="94">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-03T15:16:04+00:00</t>
+    <t>2025-05-03T16:40:31+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -88,7 +88,7 @@
 - Le patient/usager (personne physique) via Mon espace Santé, 
 - Un système de structure (dispositif, automate, appareil connecté…), 
 - Un SNR (Service Numérique Référencé), 
-author est un ensemble constitué des sous-attributs authorInstitution, ActorXDS, authorRole et authorSpecialty et ne porte pas de valeur par lui-même. </t>
+author est un ensemble constitué des sous-attributs authorInstitution , authorPerson, authorRole et authorSpecialty et ne porte pas de valeur par lui-même. </t>
   </si>
   <si>
     <t>Purpose</t>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>Constraint(s)</t>
-  </si>
-  <si>
-    <t>Mapping: null</t>
   </si>
   <si>
     <t/>
@@ -299,12 +296,6 @@
     <t>https://mos.esante.gouv.fr/NOS/JDV_J47-FunctionCode-CISIS/FHIR/JDV-J47-FunctionCode-CISIS</t>
   </si>
   <si>
-    <t>author/functionCode@displayName</t>
-  </si>
-  <si>
-    <t>Cet attribut n'a pas besoin d’être alimenté par un élément du DICOM KOS</t>
-  </si>
-  <si>
     <t>Author.specialty</t>
   </si>
   <si>
@@ -315,12 +306,6 @@
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J56-AuthorSpecialty-DMP/FHIR/JDV-J56-AuthorSpecialty-DMP</t>
-  </si>
-  <si>
-    <t>author/assignedAuthor/code@code</t>
-  </si>
-  <si>
-    <t>Cette métadonnée peut ne pas être renseignée dans le cas d’un DICOM KOS.   Si elle contient une valeur, elle devra contenir le code : 'DISPOSITIF' du JDV_J01_XdsAuthorSpecialty_CISIS</t>
   </si>
 </sst>
 </file>
@@ -625,7 +610,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL6"/>
+  <dimension ref="A1:AJ6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -669,8 +654,6 @@
     <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="28.83984375" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="146.93359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -782,12 +765,6 @@
       <c r="AJ1" t="s" s="1">
         <v>71</v>
       </c>
-      <c r="AK1" t="s" s="1">
-        <v>72</v>
-      </c>
-      <c r="AL1" t="s" s="1">
-        <v>72</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
@@ -798,26 +775,26 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s" s="2">
         <v>74</v>
       </c>
-      <c r="G2" t="s" s="2">
+      <c r="H2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="I2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="J2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="K2" t="s" s="2">
         <v>75</v>
-      </c>
-      <c r="H2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="I2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="J2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="K2" t="s" s="2">
-        <v>76</v>
       </c>
       <c r="L2" t="s" s="2">
         <v>9</v>
@@ -828,491 +805,461 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="S2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="T2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="U2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="V2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="W2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="X2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="Y2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="Z2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AA2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AB2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AC2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AD2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AE2" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AF2" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AG2" t="s" s="2">
         <v>73</v>
       </c>
-      <c r="S2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="T2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="U2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="V2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="W2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="X2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Y2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Z2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AA2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AB2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AC2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AE2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AF2" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG2" t="s" s="2">
+      <c r="AH2" t="s" s="2">
         <v>74</v>
       </c>
-      <c r="AH2" t="s" s="2">
-        <v>75</v>
-      </c>
       <c r="AI2" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AK2" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="AL2" t="s" s="2">
-        <v>7</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="I3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="J3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="K3" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="H3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="I3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="J3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="K3" t="s" s="2">
+      <c r="L3" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="L3" t="s" s="2">
-        <v>81</v>
-      </c>
       <c r="M3" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="S3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="T3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="U3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="V3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="W3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="X3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="Y3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="Z3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AA3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AB3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AC3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AD3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AE3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AF3" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AG3" t="s" s="2">
         <v>73</v>
       </c>
-      <c r="S3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="T3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="U3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="V3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="W3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="X3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Y3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="Z3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AA3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AB3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AC3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AE3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AF3" t="s" s="2">
+      <c r="AH3" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="AG3" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AH3" t="s" s="2">
-        <v>79</v>
-      </c>
       <c r="AI3" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AK3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AL3" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K4" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L4" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="L4" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="M4" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AK4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AL4" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K5" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="L5" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="L5" t="s" s="2">
+      <c r="M5" t="s" s="2">
         <v>87</v>
-      </c>
-      <c r="M5" t="s" s="2">
-        <v>88</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y5" s="2"/>
       <c r="Z5" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA5" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AB5" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AC5" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AD5" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AE5" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AF5" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AG5" t="s" s="2">
         <v>73</v>
       </c>
-      <c r="AB5" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AC5" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD5" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AE5" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AF5" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="AG5" t="s" s="2">
-        <v>79</v>
-      </c>
       <c r="AH5" t="s" s="2">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AK5" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AL5" t="s" s="2">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y6" s="2"/>
       <c r="Z6" t="s" s="2">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AA6" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AB6" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AC6" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AD6" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AE6" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AF6" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AG6" t="s" s="2">
         <v>73</v>
       </c>
-      <c r="AB6" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AC6" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD6" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AF6" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="AG6" t="s" s="2">
-        <v>74</v>
-      </c>
       <c r="AH6" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AK6" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AL6" t="s" s="2">
-        <v>98</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>